<commit_message>
Finalizaçao rotina Inner - 27/07/2022
</commit_message>
<xml_diff>
--- a/banco VAL_SCRIPT.xlsx
+++ b/banco VAL_SCRIPT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LinxAutoShop-Validação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaol\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BA8569-F6CE-4E7E-A81C-F37D684F47E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D83F1A8-6AE4-4C07-B1F2-13F2647C5825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="0" windowWidth="15375" windowHeight="7875" xr2:uid="{790B76D2-7B43-44E5-89BB-635BB147ED96}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{790B76D2-7B43-44E5-89BB-635BB147ED96}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="102">
   <si>
     <t>COD_SEQ</t>
   </si>
@@ -277,9 +277,6 @@
     <t>Numero minimo de ocorrências</t>
   </si>
   <si>
-    <t>Se o campo já está validado ou não</t>
-  </si>
-  <si>
     <t>Valores validos</t>
   </si>
   <si>
@@ -316,16 +313,34 @@
     <t>Revenda</t>
   </si>
   <si>
-    <t>PARAMETROS</t>
-  </si>
-  <si>
-    <t>VERSAO</t>
-  </si>
-  <si>
-    <t>Versão do sistema</t>
-  </si>
-  <si>
-    <t>TEXT</t>
+    <t>U_INNER1</t>
+  </si>
+  <si>
+    <t>U_INNER2</t>
+  </si>
+  <si>
+    <t>U_INNER3</t>
+  </si>
+  <si>
+    <t>U_INNER4</t>
+  </si>
+  <si>
+    <t>U_INNER5</t>
+  </si>
+  <si>
+    <t>BINARIO</t>
+  </si>
+  <si>
+    <t>Linha[]</t>
+  </si>
+  <si>
+    <t>Utilização de campos do INNER</t>
+  </si>
+  <si>
+    <t>0 (zero), 1(um) e 2 (dois)</t>
+  </si>
+  <si>
+    <t>Validação obrigatória</t>
   </si>
 </sst>
 </file>
@@ -349,7 +364,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -372,11 +387,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -389,9 +454,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0283F53C-37E3-4515-95CD-CBC33735D585}">
-  <dimension ref="B3:F62"/>
+  <dimension ref="B3:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,36 +788,40 @@
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -761,8 +835,11 @@
         <v>45</v>
       </c>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -776,8 +853,12 @@
         <v>47</v>
       </c>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <f>G5+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
@@ -791,8 +872,12 @@
         <v>46</v>
       </c>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <f>G6+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -806,8 +891,12 @@
         <v>48</v>
       </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G47" si="0">G7+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -821,8 +910,12 @@
         <v>49</v>
       </c>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -838,8 +931,12 @@
       <c r="F10" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -853,8 +950,12 @@
         <v>53</v>
       </c>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -868,8 +969,12 @@
         <v>55</v>
       </c>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
@@ -883,8 +988,12 @@
         <v>57</v>
       </c>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
@@ -898,8 +1007,12 @@
         <v>59</v>
       </c>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
@@ -913,8 +1026,12 @@
         <v>58</v>
       </c>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
@@ -928,8 +1045,12 @@
         <v>61</v>
       </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -943,8 +1064,12 @@
         <v>60</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
@@ -960,8 +1085,12 @@
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
@@ -975,8 +1104,12 @@
         <v>54</v>
       </c>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
@@ -990,8 +1123,12 @@
         <v>62</v>
       </c>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1005,8 +1142,12 @@
         <v>57</v>
       </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1020,8 +1161,12 @@
         <v>56</v>
       </c>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>18</v>
       </c>
@@ -1035,8 +1180,12 @@
         <v>58</v>
       </c>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1050,8 +1199,12 @@
         <v>63</v>
       </c>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>20</v>
       </c>
@@ -1065,8 +1218,12 @@
         <v>60</v>
       </c>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1080,25 +1237,35 @@
         <v>65</v>
       </c>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="2">
-        <v>10</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>44</v>
@@ -1107,73 +1274,91 @@
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="2">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="2">
-        <v>30</v>
-      </c>
-      <c r="E29" s="1" t="s">
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="2">
+        <v>30</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+      <c r="F30" s="1"/>
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="2">
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="2">
         <v>10</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="2">
-        <v>10</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="2">
-        <v>30</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>44</v>
@@ -1182,43 +1367,53 @@
         <v>10</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="2">
+        <v>30</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="2">
-        <v>10</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="2">
-        <v>30</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>73</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>44</v>
@@ -1227,13 +1422,17 @@
         <v>10</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>44</v>
@@ -1242,43 +1441,53 @@
         <v>10</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="2">
+        <v>30</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="2">
-        <v>30</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="2">
-        <v>10</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>44</v>
@@ -1287,252 +1496,349 @@
         <v>10</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="2">
+        <v>10</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="2">
+        <v>30</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="2">
+        <v>10</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="2">
+        <v>10</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+      <c r="F45" s="1"/>
+      <c r="G45" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D46" s="2">
         <v>99999</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
+      <c r="F46" s="1"/>
+      <c r="G46" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="9"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" s="2">
+        <v>30</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G53" s="1">
+        <f>G52+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D54" s="2">
         <v>1</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E54" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G54" s="1">
+        <f>G53+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="9"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G58" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D59" s="2">
+        <v>10</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1">
+        <f>G59+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1">
+        <f>G60+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="5">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D47" s="2">
-        <v>30</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D54" s="2">
-        <v>10</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="2">
-        <v>1</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" s="5">
-        <v>1</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D62" s="3">
-        <v>5</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F62" s="1"/>
+      <c r="G62" s="1">
+        <f>G61+1</f>
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B60:F60"/>
+  <mergeCells count="3">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B57:G57"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>